<commit_message>
added a few things to the BoM for submission and updated our internal BoM list
</commit_message>
<xml_diff>
--- a/Final BoM Internal Tracker (1).xlsx
+++ b/Final BoM Internal Tracker (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/302a7ce245808642/Documents/ECE1895/pcb design project 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ravigandhi/Documents/GitHub/ECE1895-DesignProject2-RRRK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{561AE66A-E833-4793-A7BB-8F26E6399B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF5BA7EA-E048-4A36-A85B-D451DB2A5BE8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C53FD95-BE7E-234B-9742-082743AF131A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{131D5302-907F-8C44-B725-F7ACF1A6B844}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12560" xr2:uid="{131D5302-907F-8C44-B725-F7ACF1A6B844}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
   <si>
     <t xml:space="preserve">Final BoM for Bop-it! Project </t>
   </si>
@@ -72,9 +72,6 @@
     <t>Adafruit Ultrasonic Sensor</t>
   </si>
   <si>
-    <t>To Order</t>
-  </si>
-  <si>
     <t>DigiKey: https://www.digikey.com/en/products/detail/adafruit-industries-llc/3942/9658069?s=N4IgTCBcDaIIwFYwA4C0YDsc6oHIBEQBdAXyA</t>
   </si>
   <si>
@@ -147,15 +144,9 @@
     <t>one Green/ one red</t>
   </si>
   <si>
-    <t>To order microSD</t>
-  </si>
-  <si>
     <t>Digikey: https://www.digikey.com/en/products/detail/microchip-technology/ATMEGA328P-PN/2357094</t>
   </si>
   <si>
-    <t>To order</t>
-  </si>
-  <si>
     <t>Normal Open</t>
   </si>
   <si>
@@ -187,6 +178,9 @@
   </si>
   <si>
     <t>Amazon: https://www.amazon.com/SanDisk-Ultra-UHS-I-Memory-Adapter/dp/B00M55C0NS/ref=sr_1_6?crid=32LXI5V3TMBAP&amp;dchild=1&amp;keywords=micro+sd+card&amp;qid=1635802740&amp;qsid=143-2056106-0764845&amp;s=electronics&amp;sprefix=micr%2Celectronics%2C73&amp;sr=1-6&amp;sres=B07FCMKK5X%2CB08GY8NHF2%2CB0887P21Z2%2CB00M55C0NS%2CB07K81Z6DF%2CB07P45BKN9%2CB07RV6N78T%2CB07YXJM282%2CB073JWXGNT%2CB07S5QW5V3%2CB07N7D2WBF%2CB07WJ359P6%2CB08RG38YWT%2CB07YQ5M4V4%2CB089VVP61W%2CB07G3H5RBT%2CB0834NWNZH%2CB08G81XVW4%2CB08XQ7NGG1%2CB07LBJC2D9&amp;srpt=FLASH_MEMORY</t>
+  </si>
+  <si>
+    <t>Ordered</t>
   </si>
 </sst>
 </file>
@@ -564,31 +558,31 @@
   <dimension ref="A2:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.1484375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.1484375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.84765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.6484375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6484375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.84765625" style="1"/>
+    <col min="6" max="6" width="16.6640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -605,7 +599,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -616,7 +610,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>8</v>
@@ -625,7 +619,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <f>IF(B7&lt;&gt;"", A6+1, "")</f>
         <v>2</v>
@@ -637,10 +631,13 @@
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.5">
+        <v>19</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <f t="shared" ref="A8:A57" si="0">IF(B8&lt;&gt;"", A7+1, "")</f>
         <v>3</v>
@@ -652,22 +649,22 @@
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C9" s="2">
         <v>2</v>
@@ -676,13 +673,13 @@
         <v>9</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -694,460 +691,463 @@
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2">
         <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="2">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2">
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="2">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="C14" s="2">
         <v>3</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="2">
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.5">
+        <v>38</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="2">
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="2">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="2">
         <v>2</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="2">
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C20" s="2">
         <v>4</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C21" s="2">
         <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>

</xml_diff>